<commit_message>
Modification graphique du Gantt
</commit_message>
<xml_diff>
--- a/Docs/Gantt_Projet_The_Independent_Supervisor.xlsx
+++ b/Docs/Gantt_Projet_The_Independent_Supervisor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COURS\The Independent Supervisor\git\tis\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414DBF9E-C07F-4F98-A763-4164461022BD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAFFB55-F2AD-45D6-A6C2-D3B8934486F7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -246,14 +246,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="7"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
     </font>
@@ -263,24 +255,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="42"/>
-      <color theme="7"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <b/>
@@ -306,24 +284,8 @@
       <scheme val="major"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="7"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -338,16 +300,41 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="7"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="42"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="8" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color rgb="FF735773"/>
-      <name val="Calibri"/>
+      <sz val="16"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Corbel"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="9">
@@ -356,23 +343,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="lightUp">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="lightUp">
-        <fgColor theme="7"/>
-        <bgColor theme="7" tint="0.59996337778862885"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="lightUp">
@@ -396,6 +366,24 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor theme="8" tint="0.59996337778862885"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -538,56 +526,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" applyFill="0" applyProtection="0">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" applyFill="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyProtection="0">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="6" borderId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
@@ -601,16 +589,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="2" xfId="3">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="6">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="7">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="6">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="7">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,31 +607,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="6" borderId="1" xfId="13">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="1" xfId="13">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,22 +643,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -679,88 +658,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="8" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
@@ -781,16 +751,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="5" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="5" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -815,7 +803,125 @@
     <cellStyle name="Titre 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Valeur de la période" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="8" tint="-0.499984740745262"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="8" tint="-0.499984740745262"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="8" tint="-0.499984740745262"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="8" tint="-0.499984740745262"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="8" tint="-0.499984740745262"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -868,33 +974,7 @@
       <fill>
         <patternFill patternType="lightUp">
           <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -908,19 +988,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <border>
@@ -981,33 +1048,7 @@
       <fill>
         <patternFill patternType="lightUp">
           <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
       <border>
@@ -1021,19 +1062,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <border>
@@ -1147,35 +1175,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <border>
@@ -1437,7 +1439,7 @@
   <dimension ref="B1:AO21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="84" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AQ19" sqref="AQ19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1465,13 +1467,13 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:41" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="B2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1479,37 +1481,37 @@
         <v>27</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="55"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="49"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="53" t="s">
+      <c r="Q2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="55"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="49"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="57" t="s">
+      <c r="V2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="59"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="53"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="60" t="s">
+      <c r="AA2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="62"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="56"/>
       <c r="AH2" s="16"/>
       <c r="AI2" s="18" t="s">
         <v>13</v>
@@ -1522,22 +1524,22 @@
       <c r="AO2" s="19"/>
     </row>
     <row r="3" spans="2:41" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="46" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1562,20 +1564,20 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AJ3" s="50" t="s">
+      <c r="AJ3" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="50" t="s">
+      <c r="AK3" s="44" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="65"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1660,476 +1662,476 @@
       <c r="AI4" s="3">
         <v>28</v>
       </c>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="51"/>
+      <c r="AJ4" s="45"/>
+      <c r="AK4" s="45"/>
     </row>
     <row r="5" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>1</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>2</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>1</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="60">
         <v>1</v>
       </c>
-      <c r="AJ5" s="45">
+      <c r="AJ5" s="38">
         <v>15</v>
       </c>
-      <c r="AK5" s="45">
+      <c r="AK5" s="38">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>6</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>6</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <v>6</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>6</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="60">
         <v>1</v>
       </c>
-      <c r="AJ6" s="46">
+      <c r="AJ6" s="39">
         <v>35</v>
       </c>
-      <c r="AK6" s="46">
+      <c r="AK6" s="39">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>12</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>5</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>12</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>5</v>
       </c>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="44">
+      <c r="G7" s="60">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="37">
         <v>30</v>
       </c>
-      <c r="AK7" s="44">
+      <c r="AK7" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="23">
         <f>MIN(C9,C10)</f>
         <v>11</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <f>MAX(C9+D9,C10+D10)-C8</f>
         <v>4</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="23">
         <f>MIN(E9,E10)</f>
         <v>11</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="23">
         <f>MAX(E9+F9,E10+F10)-E8</f>
         <v>4</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="61">
         <f>(G9+G10)/2</f>
         <v>0</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="28"/>
-      <c r="AD8" s="28"/>
-      <c r="AE8" s="28"/>
-      <c r="AF8" s="28"/>
-      <c r="AG8" s="28"/>
-      <c r="AH8" s="28"/>
-      <c r="AI8" s="28"/>
-      <c r="AJ8" s="48">
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="59">
         <f>AJ9+AJ10</f>
         <v>25</v>
       </c>
-      <c r="AK8" s="48">
+      <c r="AK8" s="59">
         <f>AK9+AK10</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="27">
         <v>11</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="27">
         <v>3</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="27">
         <v>11</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="27">
         <v>3</v>
       </c>
-      <c r="G9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="46">
+      <c r="G9" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="39">
         <v>20</v>
       </c>
-      <c r="AK9" s="46">
+      <c r="AK9" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="28">
         <v>13</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="28">
         <v>2</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="28">
         <v>13</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="28">
         <v>2</v>
       </c>
-      <c r="G10" s="33">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="44">
+      <c r="G10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="37">
         <v>5</v>
       </c>
-      <c r="AK10" s="44">
+      <c r="AK10" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="23">
         <f>MIN(C13,C12)</f>
         <v>13</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="23">
         <f>MAX(C13+D13,C12+D12)-C11</f>
         <v>12</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="23">
         <f>MIN(E13,E12)</f>
         <v>13</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="23">
         <f>MAX(E13+F13,E12+F12)-E11</f>
         <v>12</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="61">
         <f>(G13+G12)/2</f>
         <v>0</v>
       </c>
-      <c r="AJ11" s="47">
+      <c r="AJ11" s="58">
         <f>AJ12+AJ13+AJ14</f>
         <v>135</v>
       </c>
-      <c r="AK11" s="47">
+      <c r="AK11" s="58">
         <f>AK12+AK13+AK14</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="27">
         <v>13</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="27">
         <v>2</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="27">
         <v>13</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="27">
         <v>2</v>
       </c>
-      <c r="G12" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="46">
+      <c r="G12" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="39">
         <v>15</v>
       </c>
-      <c r="AK12" s="46">
+      <c r="AK12" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="34">
         <v>14</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="34">
         <v>11</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="34">
         <v>14</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="34">
         <v>11</v>
       </c>
-      <c r="G13" s="40">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="46">
+      <c r="G13" s="64">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="39">
         <v>80</v>
       </c>
-      <c r="AK13" s="46">
+      <c r="AK13" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="28">
         <v>18</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="28">
         <v>6</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="28">
         <v>18</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="28">
         <v>6</v>
       </c>
-      <c r="G14" s="33">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="44">
+      <c r="G14" s="63">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="37">
         <v>40</v>
       </c>
-      <c r="AK14" s="44">
+      <c r="AK14" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="23">
         <f>MIN(C16,C17,C18,C19)</f>
         <v>17</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="23">
         <f>MAX(C16+D16,C17+D17,C18+D18,C19+D19)-C15</f>
         <v>10</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="23">
         <f>MIN(E16,E17,E18,E19)</f>
         <v>17</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="23">
         <f>MAX(E16+F16,E17+F17,E18+F18,E19+F19)-E15</f>
         <v>10</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="61">
         <f>(G16+G17+G18+G19)/4</f>
         <v>0</v>
       </c>
-      <c r="AJ15" s="47">
+      <c r="AJ15" s="58">
         <f>AJ16+AJ17+AJ18+AJ19</f>
         <v>70</v>
       </c>
-      <c r="AK15" s="47">
+      <c r="AK15" s="58">
         <f>AK16+AK17+AK18+AK19</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="29">
         <v>23</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="27">
         <v>2</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="27">
         <v>23</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="27">
         <v>2</v>
       </c>
-      <c r="G16" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="46">
+      <c r="G16" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="39">
         <v>15</v>
       </c>
-      <c r="AK16" s="46">
+      <c r="AK16" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="29">
         <v>17</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="27">
         <v>9</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="27">
         <v>17</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="27">
         <v>9</v>
       </c>
-      <c r="G17" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="46">
+      <c r="G17" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="39">
         <v>30</v>
       </c>
-      <c r="AK17" s="46">
+      <c r="AK17" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="27">
         <v>25</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="27">
         <v>2</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="27">
         <v>25</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="27">
         <v>2</v>
       </c>
-      <c r="G18" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="46">
+      <c r="G18" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="39">
         <v>20</v>
       </c>
-      <c r="AK18" s="46">
+      <c r="AK18" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="27">
         <v>26</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="27">
         <v>1</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="27">
         <v>26</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="27">
         <v>1</v>
       </c>
-      <c r="G19" s="31">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="44">
+      <c r="G19" s="62">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="37">
         <v>5</v>
       </c>
-      <c r="AK19" s="44">
+      <c r="AK19" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="36">
         <v>27</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="36">
         <v>1</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="36">
         <v>27</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="36">
         <v>1</v>
       </c>
-      <c r="G20" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="42">
+      <c r="G20" s="65">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="36">
         <v>10</v>
       </c>
-      <c r="AK20" s="42">
+      <c r="AK20" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="66" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="20">
@@ -2213,14 +2215,14 @@
       <c r="AH21" s="20">
         <v>8</v>
       </c>
-      <c r="AI21" s="66">
+      <c r="AI21" s="40">
         <v>9</v>
       </c>
-      <c r="AJ21" s="49">
+      <c r="AJ21" s="57">
         <f>AJ20+AJ15+AJ11+AJ8+AJ7+AJ6+AJ5</f>
         <v>320</v>
       </c>
-      <c r="AK21" s="49">
+      <c r="AK21" s="57">
         <f>AK20+AK15+AK11+AK8+AK7+AK6+AK5</f>
         <v>37</v>
       </c>
@@ -2230,12 +2232,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AJ3:AJ4"/>
     <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="G3:G4"/>
@@ -2243,92 +2239,108 @@
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H7:AI20">
-    <cfRule type="expression" dxfId="25" priority="41">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PourcentageAccompli</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="43">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>PourcentageAccompliAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="44">
+    <cfRule type="expression" dxfId="0" priority="43">
       <formula>Réel</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="45">
+    <cfRule type="expression" dxfId="26" priority="45">
       <formula>RéelAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="46">
+    <cfRule type="expression" dxfId="25" priority="46">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="47">
+    <cfRule type="expression" dxfId="24" priority="47">
       <formula>H$4=période_sélectionnée</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="51">
+    <cfRule type="expression" dxfId="23" priority="53">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="52">
+    <cfRule type="expression" dxfId="22" priority="54">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:AI21">
-    <cfRule type="expression" dxfId="17" priority="42">
+    <cfRule type="expression" dxfId="21" priority="44">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:AI4">
-    <cfRule type="expression" dxfId="16" priority="48">
+    <cfRule type="expression" dxfId="20" priority="50">
       <formula>H$4=période_sélectionnée</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:AI5">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>PourcentageAccompli</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>PourcentageAccompliAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>Réel</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>RéelAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="17" priority="16">
       <formula>H$4=période_sélectionnée</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:AI6">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>PourcentageAccompli</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>PourcentageAccompliAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>Réel</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>RéelAuDelà</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>H$4=période_sélectionnée</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:AI8 H11:AI11 H15:AI15">
+    <cfRule type="expression" dxfId="9" priority="48">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8 H8:AI8 H11:AI11 H15:AI15">
+    <cfRule type="expression" dxfId="8" priority="49">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>